<commit_message>
thêm trạng thái hoạt động cho combo
</commit_message>
<xml_diff>
--- a/public/excel/Combo.xlsx
+++ b/public/excel/Combo.xlsx
@@ -24,28 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
-  <si>
-    <t>Winmart</t>
-  </si>
-  <si>
-    <t>10316863</t>
-  </si>
-  <si>
-    <t>TL Vỉ 2 Gôm E-017/FR</t>
-  </si>
-  <si>
-    <t>10315837</t>
-  </si>
-  <si>
-    <t>TL Bộ sáp nặn MCT - C01/DO - 16 món</t>
-  </si>
-  <si>
-    <t>10280962</t>
-  </si>
-  <si>
-    <t>TL Kéo văn phòng SC-016 hộp 20/T240</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nhóm KH</t>
   </si>
@@ -57,6 +36,21 @@
   </si>
   <si>
     <t>Barcode</t>
+  </si>
+  <si>
+    <t>Lotte</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Xóa-Phế liệu Sáp CRC Xanh lợt</t>
+  </si>
+  <si>
+    <t>8935001810308</t>
   </si>
 </sst>
 </file>
@@ -115,10 +109,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,71 +399,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3">
+        <v>90000631</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update lại file excel bảng combo và hàng tặng hàng
</commit_message>
<xml_diff>
--- a/public/excel/Combo.xlsx
+++ b/public/excel/Combo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TLG\DeliveryTracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft.public\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,22 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Nhóm KH</t>
-  </si>
-  <si>
-    <t>Mã SP</t>
-  </si>
-  <si>
-    <t>Tên SP</t>
-  </si>
-  <si>
-    <t>Barcode</t>
-  </si>
-  <si>
-    <t>Lotte</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Trạng thái</t>
   </si>
@@ -47,10 +32,22 @@
     <t>x</t>
   </si>
   <si>
-    <t>Xóa-Phế liệu Sáp CRC Xanh lợt</t>
-  </si>
-  <si>
-    <t>8935001810308</t>
+    <t>Nhóm khách hàng</t>
+  </si>
+  <si>
+    <t>Mã sản phẩm</t>
+  </si>
+  <si>
+    <t>Tên sản phẩm</t>
+  </si>
+  <si>
+    <t>Mã Barcode</t>
+  </si>
+  <si>
+    <t>Emart</t>
+  </si>
+  <si>
+    <t>Bút vẽ lên vải FM-C002 túi 12 màu</t>
   </si>
 </sst>
 </file>
@@ -68,18 +65,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB0C4DE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -92,16 +93,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -109,15 +110,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -402,49 +398,50 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="60" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3">
-        <v>90000631</v>
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>50011840</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
+      <c r="D2">
+        <v>8935001868620</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>